<commit_message>
change 'scroll down text' on all the pages
</commit_message>
<xml_diff>
--- a/Resources/Video Titles & Speaker.xlsx
+++ b/Resources/Video Titles & Speaker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dominic-my.sharepoint.com/personal/bparker_dominic_tas_edu_au/Documents/UI Design/Academic Pathways 2021/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C4E007E8-40B0-4272-9074-11E7507285B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B5FBCF0-9733-4DFD-A74B-FE7EEC05A4DC}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C4E007E8-40B0-4272-9074-11E7507285B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5F6753-E65C-48E3-8CE5-19B70DDAC4D5}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="-19720" windowWidth="24000" windowHeight="15710" xr2:uid="{AAC7FBAE-4EBB-44B0-B370-06258DFA203C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{AAC7FBAE-4EBB-44B0-B370-06258DFA203C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="95">
   <si>
     <t>Beth Gilligan</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Christian Majchrzak</t>
+  </si>
+  <si>
+    <t>Monique Brown</t>
   </si>
 </sst>
 </file>
@@ -689,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F38E7F6-B5B7-4A77-A268-36D22B723DDC}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1114,12 @@
       <c r="E33" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="F33" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">

</xml_diff>

<commit_message>
Temporary Removed All subject videos
New Principal message Video
</commit_message>
<xml_diff>
--- a/Resources/Video Titles & Speaker.xlsx
+++ b/Resources/Video Titles & Speaker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dominic-my.sharepoint.com/personal/bparker_dominic_tas_edu_au/Documents/UI Design/Academic Pathways 2021/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C4E007E8-40B0-4272-9074-11E7507285B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5F6753-E65C-48E3-8CE5-19B70DDAC4D5}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{C4E007E8-40B0-4272-9074-11E7507285B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A56DB6D6-E33B-475F-A011-916BC726F66B}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{AAC7FBAE-4EBB-44B0-B370-06258DFA203C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AAC7FBAE-4EBB-44B0-B370-06258DFA203C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="96">
   <si>
     <t>Beth Gilligan</t>
   </si>
@@ -309,9 +309,6 @@
     <t>-&gt;</t>
   </si>
   <si>
-    <t>Bad audio, messy</t>
-  </si>
-  <si>
     <t>Clumsy</t>
   </si>
   <si>
@@ -319,6 +316,12 @@
   </si>
   <si>
     <t>Monique Brown</t>
+  </si>
+  <si>
+    <t>Steve Casni</t>
+  </si>
+  <si>
+    <t>Year 9/10 Only Count</t>
   </si>
 </sst>
 </file>
@@ -350,7 +353,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -358,11 +361,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,6 +388,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F38E7F6-B5B7-4A77-A268-36D22B723DDC}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,10 +722,12 @@
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -727,8 +746,18 @@
       <c r="G1" s="2">
         <v>2021</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -747,8 +776,18 @@
       <c r="G2" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -767,8 +806,11 @@
       <c r="G4" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="7"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -782,13 +824,15 @@
         <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -801,11 +845,13 @@
       <c r="E6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -818,8 +864,13 @@
       <c r="E7" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -832,8 +883,10 @@
       <c r="E9" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -852,8 +905,10 @@
       <c r="G10" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -866,8 +921,10 @@
       <c r="E11" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -880,8 +937,13 @@
       <c r="E12" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -900,8 +962,13 @@
       <c r="G14" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -920,8 +987,12 @@
       <c r="G16" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -934,8 +1005,9 @@
       <c r="E18" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -948,8 +1020,9 @@
       <c r="E19" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -962,8 +1035,9 @@
       <c r="E20" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -976,8 +1050,12 @@
       <c r="E21" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -996,8 +1074,9 @@
       <c r="G23" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -1010,8 +1089,9 @@
       <c r="E24" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1024,8 +1104,9 @@
       <c r="E25" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1038,11 +1119,15 @@
       <c r="E26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1061,16 +1146,21 @@
       <c r="G28" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>82</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -1083,11 +1173,12 @@
       <c r="E31" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1100,8 +1191,9 @@
       <c r="E32" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1115,13 +1207,17 @@
         <v>87</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -1134,8 +1230,9 @@
       <c r="E35" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1148,11 +1245,12 @@
       <c r="E36" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1165,8 +1263,12 @@
       <c r="E37" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1179,11 +1281,12 @@
       <c r="E39" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -1196,11 +1299,12 @@
       <c r="E40" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -1213,11 +1317,12 @@
       <c r="E41" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -1230,11 +1335,12 @@
       <c r="E42" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -1247,11 +1353,15 @@
       <c r="E43" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -1264,8 +1374,9 @@
       <c r="E45" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -1278,8 +1389,9 @@
       <c r="E46" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -1292,8 +1404,9 @@
       <c r="E47" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -1306,11 +1419,12 @@
       <c r="E48" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -1320,11 +1434,12 @@
       <c r="C49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>91</v>
+      </c>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>80</v>
       </c>
@@ -1334,11 +1449,15 @@
       <c r="C50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -1348,11 +1467,12 @@
       <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1362,11 +1482,12 @@
       <c r="C53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>91</v>
+      </c>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1376,11 +1497,15 @@
       <c r="C54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>COUNTA(A2:A54)</f>
         <v>40</v>
@@ -1393,9 +1518,21 @@
         <f>COUNTA(C2:C54)</f>
         <v>41</v>
       </c>
-      <c r="H56">
-        <f>COUNTA(H2:H54)</f>
-        <v>15</v>
+      <c r="I56">
+        <f>COUNTA(I2:I54)</f>
+        <v>16</v>
+      </c>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f>COUNTA(A2, A16:A54)</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>